<commit_message>
edit tableView add admin check add userEditor
</commit_message>
<xml_diff>
--- a/cfg/lastOpened.xlsx
+++ b/cfg/lastOpened.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="43">
   <si>
     <t>Испытательное оборудование</t>
   </si>
@@ -123,55 +123,40 @@
     <t>#pointsName#</t>
   </si>
   <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>itemName2</t>
-  </si>
-  <si>
-    <t>serial</t>
-  </si>
-  <si>
-    <t>date2</t>
-  </si>
-  <si>
-    <t>time</t>
-  </si>
-  <si>
-    <t>operator2</t>
-  </si>
-  <si>
-    <t>pointsName</t>
-  </si>
-  <si>
-    <t>uViu</t>
-  </si>
-  <si>
-    <t>iViu</t>
-  </si>
-  <si>
-    <t>uMgr</t>
-  </si>
-  <si>
-    <t>rMgr</t>
-  </si>
-  <si>
-    <t>result</t>
-  </si>
-  <si>
-    <t>pointsName2</t>
-  </si>
-  <si>
-    <t>uViu2</t>
-  </si>
-  <si>
-    <t>iViu2</t>
-  </si>
-  <si>
-    <t>uMgr2</t>
-  </si>
-  <si>
-    <t>rMgr2</t>
+    <t>44</t>
+  </si>
+  <si>
+    <t>Резистор БРР-85</t>
+  </si>
+  <si>
+    <t>68461</t>
+  </si>
+  <si>
+    <t>30.05.2023</t>
+  </si>
+  <si>
+    <t>14:21:34</t>
+  </si>
+  <si>
+    <t>Тестовый оператор</t>
+  </si>
+  <si>
+    <t>Мегировка</t>
+  </si>
+  <si>
+    <t>9470</t>
+  </si>
+  <si>
+    <t>367.2</t>
+  </si>
+  <si>
+    <t>2500</t>
+  </si>
+  <si>
+    <t>6662</t>
+  </si>
+  <si>
+    <t>Неуспешно</t>
   </si>
 </sst>
 </file>
@@ -1467,26 +1452,14 @@
     </row>
     <row r="17" spans="1:1024" s="21" customFormat="1" ht="22.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="22"/>
-      <c r="B17" t="s">
-        <v>43</v>
-      </c>
+      <c r="B17" s="39"/>
       <c r="C17" s="40"/>
       <c r="D17" s="41"/>
-      <c r="E17" t="s">
-        <v>44</v>
-      </c>
-      <c r="F17" t="s">
-        <v>45</v>
-      </c>
-      <c r="G17" t="s">
-        <v>46</v>
-      </c>
-      <c r="H17" t="s">
-        <v>47</v>
-      </c>
-      <c r="I17" t="s">
-        <v>42</v>
-      </c>
+      <c r="E17" s="33"/>
+      <c r="F17" s="33"/>
+      <c r="G17" s="33"/>
+      <c r="H17" s="33"/>
+      <c r="I17" s="33"/>
       <c r="J17" s="27"/>
       <c r="K17" s="17"/>
     </row>

</xml_diff>